<commit_message>
Added sheet tracking module/class
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -335,11 +335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added **/__pycache__/ to gitignore
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="TEST_SHEET" sheetId="5" r:id="rId1"/>
+    <sheet name="TEXEL_SHEET_TRACKER" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,22 +26,64 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>descr</t>
+  </si>
+  <si>
+    <t>TEST_SHEET</t>
+  </si>
+  <si>
+    <t>first sheet added</t>
+  </si>
+  <si>
+    <t>var_name</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -53,8 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,12 +385,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upated gitignore to use compiled ignores from github boilerplate
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>sheet_name</t>
   </si>
@@ -47,10 +47,7 @@
     <t>value</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
+    <t>dollar</t>
   </si>
 </sst>
 </file>
@@ -386,7 +383,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -400,7 +397,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -447,10 +444,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -467,17 +464,6 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added function to name manager to retrieve named ranges that refer to ranges that no longer exist
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_SHEET" sheetId="5" r:id="rId1"/>
     <sheet name="TEXEL_SHEET_TRACKER" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId3"/>
     <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="YO">TEST_STANDARD_ROW!$A:$A</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>sheet_name</t>
   </si>
@@ -48,6 +51,9 @@
   </si>
   <si>
     <t>dollar</t>
+  </si>
+  <si>
+    <t>kwh</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -397,7 +403,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -432,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -464,6 +470,17 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more helper functions to aid in the handling of named ranges
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_SHEET" sheetId="5" r:id="rId1"/>
-    <sheet name="TEXEL_SHEET_TRACKER" sheetId="4" r:id="rId2"/>
-    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId3"/>
-    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId4"/>
+    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId2"/>
+    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="YO">TEST_STANDARD_ROW!$A:$A</definedName>
@@ -30,19 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>descr</t>
-  </si>
-  <si>
-    <t>TEST_SHEET</t>
-  </si>
-  <si>
-    <t>first sheet added</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>var_name</t>
   </si>
@@ -60,33 +47,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,11 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,46 +371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -448,7 +383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -460,15 +395,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -476,7 +411,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>100</v>

</xml_diff>

<commit_message>
Added more helper functions and delegated responsiblities to composed classes in the top book class
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,15 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST_SHEET" sheetId="5" r:id="rId1"/>
-    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId2"/>
-    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId3"/>
+    <sheet name="TEST_SHEET_TXL_ROW" sheetId="11" r:id="rId1"/>
+    <sheet name="TXL_SHEET_TRACKER" sheetId="10" r:id="rId2"/>
+    <sheet name="TEST_SHEET" sheetId="5" r:id="rId3"/>
+    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId4"/>
+    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="YO">TEST_STANDARD_ROW!$A:$A</definedName>
+    <definedName name="TEST_NAME_FOR_NBK">TEST_SHEET_TXL_ROW!$I$13</definedName>
+    <definedName name="TEST_SCALAR_INPUT__dollar">TEST_SCALAR_INPUT!$B$2</definedName>
+    <definedName name="TEST_SCALAR_INPUT__kwh">TEST_SCALAR_INPUT!$B$3</definedName>
+    <definedName name="TESTOTHER_NAME">TEST_SHEET_TXL_ROW!$O$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>var_name</t>
   </si>
@@ -41,6 +46,39 @@
   </si>
   <si>
     <t>kwh</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>descr</t>
+  </si>
+  <si>
+    <t>sheet_type</t>
+  </si>
+  <si>
+    <t>TEST_SCALAR_INPUT</t>
+  </si>
+  <si>
+    <t>A Test worksheet with scalar inputs</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yellow</t>
   </si>
 </sst>
 </file>
@@ -55,12 +93,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,7 +405,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -371,10 +416,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="1.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -383,12 +471,67 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Name manager now handles adding, renaming, and swapping of named ranges
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_SHEET_TXL_ROW" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>var_name</t>
   </si>
@@ -57,6 +57,9 @@
     <t>sheet_type</t>
   </si>
   <si>
+    <t>TEST_STANDARD_ROW</t>
+  </si>
+  <si>
     <t>TEST_SCALAR_INPUT</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
   </si>
   <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>Standard Row tab for testing</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -416,15 +422,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="1.875" bestFit="1" customWidth="1"/>
@@ -443,13 +449,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -475,18 +492,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -494,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -502,7 +519,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -510,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -518,7 +535,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -530,11 +547,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Added subprocess that deletes all named ranges with references errors before a naming update.
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,20 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST_SHEET_TXL_ROW" sheetId="11" r:id="rId1"/>
-    <sheet name="TXL_SHEET_TRACKER" sheetId="10" r:id="rId2"/>
-    <sheet name="TEST_SHEET" sheetId="5" r:id="rId3"/>
-    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId4"/>
-    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId5"/>
+    <sheet name="TXL_SHEET_TRACKER" sheetId="13" r:id="rId1"/>
+    <sheet name="TEST_SHEET" sheetId="5" r:id="rId2"/>
+    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId3"/>
+    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="TEST_NAME_FOR_NBK">TEST_SHEET_TXL_ROW!$I$13</definedName>
     <definedName name="TEST_SCALAR_INPUT__dollar">TEST_SCALAR_INPUT!$B$2</definedName>
     <definedName name="TEST_SCALAR_INPUT__kwh">TEST_SCALAR_INPUT!$B$3</definedName>
-    <definedName name="TESTOTHER_NAME">TEST_SHEET_TXL_ROW!$O$12</definedName>
+    <definedName name="TEST_STANDARD_ROW__index">TEST_STANDARD_ROW!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>var_name</t>
   </si>
@@ -60,31 +58,13 @@
     <t>TEST_STANDARD_ROW</t>
   </si>
   <si>
-    <t>TEST_SCALAR_INPUT</t>
-  </si>
-  <si>
-    <t>A Test worksheet with scalar inputs</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>Standard Row tab for testing</t>
+    <t>sheet_index</t>
+  </si>
+  <si>
+    <t>Sheet to test standard row sheet</t>
   </si>
 </sst>
 </file>
@@ -408,10 +388,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f ca="1">_xlfn.SHEET(TEST_STANDARD_ROW!$A$1)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -420,122 +450,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="1.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -543,12 +490,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added to SheetTracker so that sheets that no longer exist are removed and any renames that occur after tracking will be updated automatically using the SHEET function of excel to keep a permanent reference
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -13,14 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="TXL_SHEET_TRACKER" sheetId="13" r:id="rId1"/>
-    <sheet name="TEST_SHEET" sheetId="5" r:id="rId2"/>
-    <sheet name="TEST_STANDARD_ROW" sheetId="3" r:id="rId3"/>
-    <sheet name="TEST_SCALAR_INPUT" sheetId="9" r:id="rId4"/>
+    <sheet name="TEST_SCALAR" sheetId="9" r:id="rId2"/>
+    <sheet name="TEST_SHEET" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="TEST_SCALAR_INPUT__dollar">TEST_SCALAR_INPUT!$B$2</definedName>
-    <definedName name="TEST_SCALAR_INPUT__kwh">TEST_SCALAR_INPUT!$B$3</definedName>
-    <definedName name="TEST_STANDARD_ROW__index">TEST_STANDARD_ROW!$A:$A</definedName>
+    <definedName name="TEST_SCALAR__dollar">TEST_SCALAR!$B$2</definedName>
+    <definedName name="TEST_SCALAR__kwh">TEST_SCALAR!$B$3</definedName>
+    <definedName name="TEST_SCALAR__value">TEST_SCALAR!$B:$B</definedName>
+    <definedName name="TEST_SCALAR__var_name">TEST_SCALAR!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>var_name</t>
   </si>
@@ -55,16 +55,13 @@
     <t>sheet_type</t>
   </si>
   <si>
-    <t>TEST_STANDARD_ROW</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
     <t>sheet_index</t>
   </si>
   <si>
     <t>Sheet to test standard row sheet</t>
+  </si>
+  <si>
+    <t>TEST_SCALAR</t>
   </si>
 </sst>
 </file>
@@ -391,12 +388,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
@@ -413,22 +410,21 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <f ca="1">_xlfn.SHEET(TEST_STANDARD_ROW!$A$1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -438,64 +434,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -530,4 +472,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added coloring for input and column calc tabs. Need to add it to the updating process
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="TXL_SHEET_TRACKER" sheetId="13" r:id="rId1"/>
+    <sheet name="TXL_SHEET_TRACKER" sheetId="21" r:id="rId1"/>
     <sheet name="TEST_SCALAR" sheetId="9" r:id="rId2"/>
-    <sheet name="TEST_SHEET" sheetId="5" r:id="rId3"/>
+    <sheet name="TEST_SHEET_FOR_COLORING" sheetId="22" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="TEST_SCALAR__dollar">TEST_SCALAR!$B$2</definedName>
-    <definedName name="TEST_SCALAR__kwh">TEST_SCALAR!$B$3</definedName>
+    <definedName name="TEST_SCALAR__dollar">TEST_SCALAR!$B$3</definedName>
+    <definedName name="TEST_SCALAR__kwh">TEST_SCALAR!$B$2</definedName>
     <definedName name="TEST_SCALAR__value">TEST_SCALAR!$B:$B</definedName>
     <definedName name="TEST_SCALAR__var_name">TEST_SCALAR!$A:$A</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>var_name</t>
   </si>
@@ -62,21 +62,42 @@
   </si>
   <si>
     <t>TEST_SCALAR</t>
+  </si>
+  <si>
+    <t>test_index_a</t>
+  </si>
+  <si>
+    <t>test_index_b</t>
+  </si>
+  <si>
+    <t>first_calc</t>
+  </si>
+  <si>
+    <t>first_input</t>
+  </si>
+  <si>
+    <t>second_calc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +107,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -102,9 +135,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,16 +429,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -414,17 +457,62 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <f ca="1">_xlfn.SHEET(TEST_SCALAR!$A$1)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -432,58 +520,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="2">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="2">
+        <f>A2*B2</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E2" s="2">
+        <f>C2+D2</f>
         <v>3</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Linked coloring to TexlBook class
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,18 +9,50 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="TXL_SHEET_TRACKER" sheetId="21" r:id="rId1"/>
+    <sheet name="TEST_SHEET_FOR_COLORING" sheetId="22" r:id="rId1"/>
     <sheet name="TEST_SCALAR" sheetId="9" r:id="rId2"/>
-    <sheet name="TEST_SHEET_FOR_COLORING" sheetId="22" r:id="rId3"/>
+    <sheet name="TEST_LONG_COLUMN_SHEET" sheetId="23" r:id="rId3"/>
+    <sheet name="TXL_SHEET_TRACKER" sheetId="21" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="TEST_LONG_COLUMN_SHEET__a">TEST_LONG_COLUMN_SHEET!$A:$A</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__b">TEST_LONG_COLUMN_SHEET!$B:$B</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__c">TEST_LONG_COLUMN_SHEET!$C:$C</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__d">TEST_LONG_COLUMN_SHEET!$D:$D</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__e">TEST_LONG_COLUMN_SHEET!$E:$E</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__f">TEST_LONG_COLUMN_SHEET!$F:$F</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__g">TEST_LONG_COLUMN_SHEET!$G:$G</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__h">TEST_LONG_COLUMN_SHEET!$H:$H</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__i">TEST_LONG_COLUMN_SHEET!$I:$I</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__j">TEST_LONG_COLUMN_SHEET!$J:$J</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__k">TEST_LONG_COLUMN_SHEET!$K:$K</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__l">TEST_LONG_COLUMN_SHEET!$L:$L</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__m">TEST_LONG_COLUMN_SHEET!$M:$M</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__n">TEST_LONG_COLUMN_SHEET!$N:$N</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__o">TEST_LONG_COLUMN_SHEET!$O:$O</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__p">TEST_LONG_COLUMN_SHEET!$P:$P</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__q">TEST_LONG_COLUMN_SHEET!$Q:$Q</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__r">TEST_LONG_COLUMN_SHEET!$R:$R</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__s">TEST_LONG_COLUMN_SHEET!$S:$S</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__t">TEST_LONG_COLUMN_SHEET!$T:$T</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__u">TEST_LONG_COLUMN_SHEET!$U:$U</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__v">TEST_LONG_COLUMN_SHEET!$V:$V</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__w">TEST_LONG_COLUMN_SHEET!$W:$W</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__x">TEST_LONG_COLUMN_SHEET!$X:$X</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__y">TEST_LONG_COLUMN_SHEET!$Y:$Y</definedName>
+    <definedName name="TEST_LONG_COLUMN_SHEET__z">TEST_LONG_COLUMN_SHEET!$Z:$Z</definedName>
     <definedName name="TEST_SCALAR__dollar">TEST_SCALAR!$B$3</definedName>
     <definedName name="TEST_SCALAR__kwh">TEST_SCALAR!$B$2</definedName>
     <definedName name="TEST_SCALAR__value">TEST_SCALAR!$B:$B</definedName>
     <definedName name="TEST_SCALAR__var_name">TEST_SCALAR!$A:$A</definedName>
+    <definedName name="TEST_SHEET_FOR_COLORING__first_calc">TEST_SHEET_FOR_COLORING!$C:$C</definedName>
+    <definedName name="TEST_SHEET_FOR_COLORING__first_input">TEST_SHEET_FOR_COLORING!$D:$D</definedName>
+    <definedName name="TEST_SHEET_FOR_COLORING__second_calc">TEST_SHEET_FOR_COLORING!$E:$E</definedName>
+    <definedName name="TEST_SHEET_FOR_COLORING__test_index_a">TEST_SHEET_FOR_COLORING!$A:$A</definedName>
+    <definedName name="TEST_SHEET_FOR_COLORING__test_index_b">TEST_SHEET_FOR_COLORING!$B:$B</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>var_name</t>
   </si>
@@ -77,6 +109,96 @@
   </si>
   <si>
     <t>second_calc</t>
+  </si>
+  <si>
+    <t>TEST_SHEET_FOR_COLORING</t>
+  </si>
+  <si>
+    <t>Sheet to test coloring of column cals</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>TEST_LONG_COLUMN_SHEET</t>
+  </si>
+  <si>
+    <t>Column sheet with more columns to color</t>
   </si>
 </sst>
 </file>
@@ -135,8 +257,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,53 +550,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="2"/>
+    <col min="1" max="2" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <f ca="1">_xlfn.SHEET(TEST_SCALAR!$A$1)</f>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <f>A2*B2</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <f>C2+D2</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -482,36 +611,36 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
     </row>
@@ -522,58 +651,257 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>14</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <v>17</v>
+      </c>
+      <c r="R2">
+        <v>18</v>
+      </c>
+      <c r="S2">
+        <v>19</v>
+      </c>
+      <c r="T2">
+        <v>20</v>
+      </c>
+      <c r="U2">
+        <v>21</v>
+      </c>
+      <c r="V2">
+        <v>22</v>
+      </c>
+      <c r="W2">
+        <v>23</v>
+      </c>
+      <c r="X2">
+        <v>24</v>
+      </c>
+      <c r="Y2">
+        <v>25</v>
+      </c>
+      <c r="Z2">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="19.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f ca="1">_xlfn.SHEET(TEST_SCALAR!$A$1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <f>A2*B2</f>
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="D3" s="3">
+        <f ca="1">_xlfn.SHEET(TEST_SHEET_FOR_COLORING!$A$1)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <f>C2+D2</f>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <f ca="1">_xlfn.SHEET(TEST_LONG_COLUMN_SHEET!$A$1)</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added methods to color tabs
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -9,45 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_SHEET_FOR_COLORING" sheetId="22" r:id="rId1"/>
-    <sheet name="TEST_SCALAR" sheetId="9" r:id="rId2"/>
-    <sheet name="TEST_LONG_COLUMN_SHEET" sheetId="23" r:id="rId3"/>
-    <sheet name="TXL_SHEET_TRACKER" sheetId="21" r:id="rId4"/>
+    <sheet name="TEST_SCALAR_LOLOL" sheetId="9" r:id="rId2"/>
+    <sheet name="TXL_SHEET_TRACKER" sheetId="21" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="TEST_LONG_COLUMN_SHEET__a">TEST_LONG_COLUMN_SHEET!$A:$A</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__b">TEST_LONG_COLUMN_SHEET!$B:$B</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__c">TEST_LONG_COLUMN_SHEET!$C:$C</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__d">TEST_LONG_COLUMN_SHEET!$D:$D</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__e">TEST_LONG_COLUMN_SHEET!$E:$E</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__f">TEST_LONG_COLUMN_SHEET!$F:$F</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__g">TEST_LONG_COLUMN_SHEET!$G:$G</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__h">TEST_LONG_COLUMN_SHEET!$H:$H</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__i">TEST_LONG_COLUMN_SHEET!$I:$I</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__j">TEST_LONG_COLUMN_SHEET!$J:$J</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__k">TEST_LONG_COLUMN_SHEET!$K:$K</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__l">TEST_LONG_COLUMN_SHEET!$L:$L</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__m">TEST_LONG_COLUMN_SHEET!$M:$M</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__n">TEST_LONG_COLUMN_SHEET!$N:$N</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__o">TEST_LONG_COLUMN_SHEET!$O:$O</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__p">TEST_LONG_COLUMN_SHEET!$P:$P</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__q">TEST_LONG_COLUMN_SHEET!$Q:$Q</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__r">TEST_LONG_COLUMN_SHEET!$R:$R</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__s">TEST_LONG_COLUMN_SHEET!$S:$S</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__t">TEST_LONG_COLUMN_SHEET!$T:$T</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__u">TEST_LONG_COLUMN_SHEET!$U:$U</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__v">TEST_LONG_COLUMN_SHEET!$V:$V</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__w">TEST_LONG_COLUMN_SHEET!$W:$W</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__x">TEST_LONG_COLUMN_SHEET!$X:$X</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__y">TEST_LONG_COLUMN_SHEET!$Y:$Y</definedName>
-    <definedName name="TEST_LONG_COLUMN_SHEET__z">TEST_LONG_COLUMN_SHEET!$Z:$Z</definedName>
-    <definedName name="TEST_SCALAR__dollar">TEST_SCALAR!$B$3</definedName>
-    <definedName name="TEST_SCALAR__kwh">TEST_SCALAR!$B$2</definedName>
-    <definedName name="TEST_SCALAR__value">TEST_SCALAR!$B:$B</definedName>
-    <definedName name="TEST_SCALAR__var_name">TEST_SCALAR!$A:$A</definedName>
+    <definedName name="TEST_SCALAR__value">TEST_SCALAR_LOLOL!$B:$B</definedName>
+    <definedName name="TEST_SCALAR__var_name">TEST_SCALAR_LOLOL!$A:$A</definedName>
+    <definedName name="TEST_SCALAR_LOLOL__dollar">TEST_SCALAR_LOLOL!$B$3</definedName>
+    <definedName name="TEST_SCALAR_LOLOL__kwh">TEST_SCALAR_LOLOL!$B$2</definedName>
     <definedName name="TEST_SHEET_FOR_COLORING__first_calc">TEST_SHEET_FOR_COLORING!$C:$C</definedName>
     <definedName name="TEST_SHEET_FOR_COLORING__first_input">TEST_SHEET_FOR_COLORING!$D:$D</definedName>
     <definedName name="TEST_SHEET_FOR_COLORING__second_calc">TEST_SHEET_FOR_COLORING!$E:$E</definedName>
@@ -64,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>var_name</t>
   </si>
@@ -93,9 +66,6 @@
     <t>Sheet to test standard row sheet</t>
   </si>
   <si>
-    <t>TEST_SCALAR</t>
-  </si>
-  <si>
     <t>test_index_a</t>
   </si>
   <si>
@@ -117,88 +87,7 @@
     <t>Sheet to test coloring of column cals</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>TEST_LONG_COLUMN_SHEET</t>
-  </si>
-  <si>
-    <t>Column sheet with more columns to color</t>
+    <t>TEST_SCALAR_LOLOL</t>
   </si>
 </sst>
 </file>
@@ -219,7 +108,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +133,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -257,25 +152,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFACBEE2"/>
+      <color rgb="FFC4DCEA"/>
+      <color rgb="FFD8E9F4"/>
+      <color rgb="FFCCFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -550,36 +452,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2">
+    <tabColor rgb="FFBDD7EE"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -603,15 +509,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3">
+    <tabColor rgb="FFF8CBAD"/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -621,10 +531,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -651,213 +561,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2">
-        <v>11</v>
-      </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2">
-        <v>13</v>
-      </c>
-      <c r="N2">
-        <v>14</v>
-      </c>
-      <c r="O2">
-        <v>15</v>
-      </c>
-      <c r="P2">
-        <v>16</v>
-      </c>
-      <c r="Q2">
-        <v>17</v>
-      </c>
-      <c r="R2">
-        <v>18</v>
-      </c>
-      <c r="S2">
-        <v>19</v>
-      </c>
-      <c r="T2">
-        <v>20</v>
-      </c>
-      <c r="U2">
-        <v>21</v>
-      </c>
-      <c r="V2">
-        <v>22</v>
-      </c>
-      <c r="W2">
-        <v>23</v>
-      </c>
-      <c r="X2">
-        <v>24</v>
-      </c>
-      <c r="Y2">
-        <v>25</v>
-      </c>
-      <c r="Z2">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.25" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -866,16 +602,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <f ca="1">_xlfn.SHEET(TEST_SCALAR!$A$1)</f>
+        <f ca="1">_xlfn.SHEET(TEST_SCALAR_LOLOL!$A$1)</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -883,21 +619,6 @@
       <c r="D3" s="3">
         <f ca="1">_xlfn.SHEET(TEST_SHEET_FOR_COLORING!$A$1)</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <f ca="1">_xlfn.SHEET(TEST_LONG_COLUMN_SHEET!$A$1)</f>
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more formatting options
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -12,15 +12,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST_SHEET_FOR_COLORING" sheetId="22" r:id="rId1"/>
-    <sheet name="TEST_SCALAR_LOLOL" sheetId="9" r:id="rId2"/>
-    <sheet name="TXL_SHEET_TRACKER" sheetId="21" r:id="rId3"/>
+    <sheet name="TXL_SHEET_TRACKER" sheetId="27" r:id="rId1"/>
+    <sheet name="TEST_SHEET_FOR_COLORING" sheetId="22" r:id="rId2"/>
+    <sheet name="TEST_SCALAR" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="TEST_SCALAR__value">TEST_SCALAR_LOLOL!$B:$B</definedName>
-    <definedName name="TEST_SCALAR__var_name">TEST_SCALAR_LOLOL!$A:$A</definedName>
-    <definedName name="TEST_SCALAR_LOLOL__dollar">TEST_SCALAR_LOLOL!$B$3</definedName>
-    <definedName name="TEST_SCALAR_LOLOL__kwh">TEST_SCALAR_LOLOL!$B$2</definedName>
+    <definedName name="TEST_SCALAR__value">TEST_SCALAR!$B:$B</definedName>
+    <definedName name="TEST_SCALAR__var_name">TEST_SCALAR!$A:$A</definedName>
+    <definedName name="TEST_SCALAR_LOLOL__dollar">TEST_SCALAR!$B$3</definedName>
+    <definedName name="TEST_SCALAR_LOLOL__kwh">TEST_SCALAR!$B$2</definedName>
     <definedName name="TEST_SHEET_FOR_COLORING__first_calc">TEST_SHEET_FOR_COLORING!$C:$C</definedName>
     <definedName name="TEST_SHEET_FOR_COLORING__first_input">TEST_SHEET_FOR_COLORING!$D:$D</definedName>
     <definedName name="TEST_SHEET_FOR_COLORING__second_calc">TEST_SHEET_FOR_COLORING!$E:$E</definedName>
@@ -66,6 +66,9 @@
     <t>Sheet to test standard row sheet</t>
   </si>
   <si>
+    <t>TEST_SCALAR</t>
+  </si>
+  <si>
     <t>test_index_a</t>
   </si>
   <si>
@@ -85,16 +88,13 @@
   </si>
   <si>
     <t>Sheet to test coloring of column cals</t>
-  </si>
-  <si>
-    <t>TEST_SCALAR_LOLOL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +107,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFEDF2F4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +143,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF355185"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDF2F4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -162,6 +181,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -452,13 +475,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7">
+    <tabColor rgb="FF355185"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <f ca="1">_xlfn.SHEET(TEST_SCALAR!$A$1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <f ca="1">_xlfn.SHEET(TEST_SHEET_FOR_COLORING!$A$1)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFBDD7EE"/>
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -473,19 +565,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -513,7 +605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFF8CBAD"/>
@@ -521,7 +613,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -557,72 +649,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <f ca="1">_xlfn.SHEET(TEST_SCALAR_LOLOL!$A$1)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <f ca="1">_xlfn.SHEET(TEST_SHEET_FOR_COLORING!$A$1)</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>